<commit_message>
improved generation for new shacl shapes
</commit_message>
<xml_diff>
--- a/cpsv-ap.xlsx
+++ b/cpsv-ap.xlsx
@@ -767,9 +767,7 @@
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="6" max="8" width="22.5703125" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
     <col min="10" max="10" width="22.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
@@ -1474,8 +1472,7 @@
     <col min="2" max="2" width="36.42578125" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="5" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1698,8 +1695,7 @@
     <col min="2" max="2" width="39.85546875" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="5" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" customWidth="1"/>
@@ -2545,8 +2541,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="2" max="3" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2753,8 +2748,7 @@
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="5" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3193,8 +3187,7 @@
     <col min="2" max="2" width="36.42578125" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="5" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3631,23 +3624,18 @@
     <col min="8" max="8" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" customWidth="1"/>
+    <col min="11" max="13" width="22.5703125" customWidth="1"/>
     <col min="14" max="14" width="16.85546875" customWidth="1"/>
     <col min="15" max="15" width="20.28515625" customWidth="1"/>
     <col min="16" max="16" width="19.140625" customWidth="1"/>
     <col min="17" max="17" width="16.85546875" customWidth="1"/>
     <col min="18" max="18" width="18" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" customWidth="1"/>
+    <col min="19" max="20" width="14.5703125" customWidth="1"/>
     <col min="21" max="21" width="20.28515625" customWidth="1"/>
     <col min="22" max="22" width="15.7109375" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" customWidth="1"/>
-    <col min="24" max="24" width="14.5703125" customWidth="1"/>
+    <col min="23" max="24" width="14.5703125" customWidth="1"/>
     <col min="25" max="25" width="11" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" customWidth="1"/>
-    <col min="27" max="27" width="13.42578125" customWidth="1"/>
+    <col min="26" max="27" width="13.42578125" customWidth="1"/>
     <col min="28" max="28" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3930,8 +3918,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="2" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
@@ -4158,8 +4145,7 @@
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="6" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5468,8 +5454,7 @@
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="6" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>